<commit_message>
creacion de objetos maquinas
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaiza\Documents\curso4\dp\prac_final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaiza\Documents\curso4\dp\prac_final\PPG-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40BB4FA-DC39-4646-8416-68BC28F8DDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54899312-26FC-49E2-A71B-C39F988161D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="828" windowWidth="12396" windowHeight="8964" xr2:uid="{7B943A46-EE26-45A5-A415-8CC152017EBD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7B943A46-EE26-45A5-A415-8CC152017EBD}"/>
   </bookViews>
   <sheets>
     <sheet name="prod" sheetId="1" r:id="rId1"/>
@@ -2055,8 +2055,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:CC277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5806,7 +5806,9 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5840,70 +5842,70 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1400</v>
+        <v>347</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5000</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>332</v>
+      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="5">
-        <v>3.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="D3" s="2">
-        <v>1400</v>
+        <v>8000</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="F3" s="5"/>
+        <v>333</v>
+      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="5">
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1400</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="F4" s="5"/>
+        <v>340</v>
+      </c>
+      <c r="D4" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="5">
-        <v>3.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>93</v>
@@ -5912,19 +5914,19 @@
         <v>340</v>
       </c>
       <c r="D5" s="6">
-        <v>4000</v>
+        <v>10000</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>93</v>
@@ -5933,14 +5935,14 @@
         <v>340</v>
       </c>
       <c r="D6" s="6">
-        <v>8000</v>
+        <v>10000</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="5">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -5954,56 +5956,56 @@
         <v>340</v>
       </c>
       <c r="D7" s="6">
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="5">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D8" s="6">
         <v>4000</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="5">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D9" s="6">
-        <v>8000</v>
+        <v>4000</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="5">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -6014,17 +6016,17 @@
         <v>93</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D10" s="6">
-        <v>20000</v>
+        <v>8000</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -6038,10 +6040,10 @@
         <v>340</v>
       </c>
       <c r="D11" s="6">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="5">
@@ -6050,7 +6052,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>93</v>
@@ -6071,7 +6073,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>93</v>
@@ -6079,57 +6081,57 @@
       <c r="C13" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D13" s="6">
-        <v>10000</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="5">
-        <v>1.25</v>
-      </c>
+      <c r="D13" s="2">
+        <v>25000</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="D14" s="6">
-        <v>4000</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>329</v>
+        <v>1500</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>344</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="5">
-        <v>1.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="D15" s="6">
-        <v>8000</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>359</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1400</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -6140,17 +6142,17 @@
         <v>93</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="D16" s="6">
-        <v>20000</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>359</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1400</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F16" s="5"/>
       <c r="G16" s="5">
-        <v>1</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -6161,85 +6163,85 @@
         <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D17" s="6">
-        <v>4000</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>359</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1400</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F17" s="5"/>
       <c r="G17" s="5">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D18" s="6">
-        <v>8000</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="F18" s="7"/>
+        <v>341</v>
+      </c>
+      <c r="D18" s="2">
+        <v>18001</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="F18" s="5"/>
       <c r="G18" s="5">
-        <v>0.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D19" s="6">
-        <v>10000</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>327</v>
+        <v>5000</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>346</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="5">
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>154</v>
+        <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>341</v>
       </c>
       <c r="D20" s="6">
-        <v>4000</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>329</v>
+        <v>7200</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>349</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>93</v>
@@ -6248,19 +6250,19 @@
         <v>341</v>
       </c>
       <c r="D21" s="6">
-        <v>8000</v>
+        <v>20000</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>154</v>
+        <v>91</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>93</v>
@@ -6281,149 +6283,149 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>107</v>
+        <v>154</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D23" s="2">
-        <v>11999</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>341</v>
+      </c>
+      <c r="D23" s="6">
+        <v>20000</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="F23" s="7"/>
       <c r="G23" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>93</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D24" s="2">
-        <v>25000</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F24" s="5">
-        <v>1</v>
-      </c>
-      <c r="G24" s="5"/>
+        <v>341</v>
+      </c>
+      <c r="D24" s="6">
+        <v>4000</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="5">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="D25" s="6">
-        <v>5200</v>
+        <v>4000</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="7">
-        <v>6</v>
-      </c>
-      <c r="G25" s="5"/>
+        <v>329</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="5">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="D26" s="6">
-        <v>5200</v>
+        <v>4000</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F26" s="7">
-        <v>6</v>
-      </c>
-      <c r="G26" s="5"/>
+        <v>329</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="5">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="D27" s="6">
-        <v>5200</v>
+        <v>8000</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="7">
-        <v>6</v>
-      </c>
-      <c r="G27" s="5"/>
+        <v>330</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="5">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="D28" s="6">
-        <v>1500</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>344</v>
+        <v>8000</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>330</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="5">
-        <v>6</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D29" s="6">
-        <v>5000</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>345</v>
+        <v>8000</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>330</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -6431,20 +6433,20 @@
         <v>87</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="D30" s="6">
-        <v>5000</v>
+        <v>359</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1000</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="F30" s="7"/>
+        <v>353</v>
+      </c>
+      <c r="F30" s="8"/>
       <c r="G30" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -6452,18 +6454,18 @@
         <v>87</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D31" s="6">
-        <v>5000</v>
+        <v>359</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4400</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="F31" s="7"/>
+        <v>354</v>
+      </c>
+      <c r="F31" s="8"/>
       <c r="G31" s="5">
         <v>1</v>
       </c>
@@ -6473,19 +6475,21 @@
         <v>87</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D32" s="6">
-        <v>8000</v>
+        <v>359</v>
+      </c>
+      <c r="D32" s="2">
+        <v>500</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="5"/>
+        <v>352</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -6495,17 +6499,17 @@
         <v>88</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="D33" s="6">
-        <v>7200</v>
+        <v>340</v>
+      </c>
+      <c r="D33" s="2">
+        <v>20001</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>350</v>
+      </c>
+      <c r="F33" s="5"/>
       <c r="G33" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -6516,17 +6520,17 @@
         <v>88</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="D34" s="2">
-        <v>8000</v>
+        <v>340</v>
+      </c>
+      <c r="D34" s="6">
+        <v>5000</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>333</v>
+        <v>345</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -6539,106 +6543,108 @@
       <c r="C35" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D35" s="2">
-        <v>20001</v>
+      <c r="D35" s="6">
+        <v>8000</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5">
-        <v>4</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D36" s="2">
-        <v>18001</v>
+        <v>11999</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D37" s="2">
-        <v>500</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F37" s="8"/>
-      <c r="G37" s="5">
-        <v>1</v>
-      </c>
+      <c r="D37" s="6">
+        <v>5200</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="7">
+        <v>6</v>
+      </c>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D38" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>353</v>
-      </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="5">
-        <v>1</v>
-      </c>
+      <c r="D38" s="6">
+        <v>5200</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="7">
+        <v>6</v>
+      </c>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D39" s="2">
-        <v>4400</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="5">
-        <v>1</v>
-      </c>
+      <c r="D39" s="6">
+        <v>5200</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="7">
+        <v>6</v>
+      </c>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C40" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G39" xr:uid="{67097983-BA14-47B5-A6B2-37DA8E8B5179}"/>
+  <autoFilter ref="A1:G39" xr:uid="{67097983-BA14-47B5-A6B2-37DA8E8B5179}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G39">
+      <sortCondition ref="E1:E39"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6649,7 +6655,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>